<commit_message>
Fix: Ajuste de validador e insert ofertas PH, NPH y Rural
</commit_message>
<xml_diff>
--- a/src/files/EJEMPLO_FORMATO_MERCADO_OBSERVATORIO_INMOBILIARIO_NACIONAL.xlsx
+++ b/src/files/EJEMPLO_FORMATO_MERCADO_OBSERVATORIO_INMOBILIARIO_NACIONAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://danegovco-my.sharepoint.com/personal/pagoenagac_dane_gov_co/Documents/Documentos/PAGOENAGAC/02_Observatorio Inmobiliario - OIN/01_Cargues Observadores/Formatos - instructivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{9A1D7074-A131-4087-9D51-A373EB1C5D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D99B3FD-3691-4F87-8A3F-0B95BBA50556}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{9A1D7074-A131-4087-9D51-A373EB1C5D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F26C8CFA-F316-4B14-B393-0FFF6F70D005}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" xr2:uid="{7AEC964B-7FBA-4D6E-B96B-7AAA67EE11BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7AEC964B-7FBA-4D6E-B96B-7AAA67EE11BC}"/>
   </bookViews>
   <sheets>
     <sheet name="PH" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="93">
   <si>
     <t>ID_OFERTA_PH</t>
   </si>
@@ -158,12 +158,6 @@
     <t>TIPO_TIPOLOGIA</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Dominio</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>178956789123</t>
   </si>
   <si>
-    <t>Vacio</t>
-  </si>
-  <si>
     <t>11001</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
   </si>
   <si>
     <t>VR_M2_TERRENO</t>
-  </si>
-  <si>
-    <t>11001011000250034001</t>
   </si>
   <si>
     <t>110010110001700250034001000000</t>
@@ -388,28 +376,46 @@
   <si>
     <t xml:space="preserve">El campo puede estar diligenciado o no. </t>
   </si>
+  <si>
+    <t>Texto</t>
+  </si>
+  <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>BDU0001CMJD</t>
+  </si>
+  <si>
+    <t>BDU0001KPJB</t>
+  </si>
+  <si>
+    <t>BCY0001SXJB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="16">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;\ * #,##0_);_(&quot;$&quot;\ * \(#,##0\);_(&quot;$&quot;\ * &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="177" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ "/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;\ #,##0.00;[Red]&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="179" formatCode="0.000"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;\ * #,##0_);_(&quot;$&quot;\ * \(#,##0\);_(&quot;$&quot;\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="172" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="173" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ "/>
+    <numFmt numFmtId="174" formatCode="&quot;$&quot;\ #,##0.00;[Red]&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="175" formatCode="0.000"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -963,13 +969,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1019,19 +1025,19 @@
     <xf numFmtId="0" fontId="12" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1040,8 +1046,8 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1051,31 +1057,31 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="174" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -1084,7 +1090,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="175" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyFill="0"/>
@@ -1115,27 +1121,27 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="27" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1158,9 +1164,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="156"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="26" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="27" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1207,13 +1210,13 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1228,11 +1231,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="26" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="27" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="27" fillId="26" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="174">
@@ -1314,8 +1335,8 @@
     <cellStyle name="Heading 2" xfId="85" xr:uid="{6CAAA471-A847-4956-B6F2-F1B66EE7AE12}"/>
     <cellStyle name="Heading 3" xfId="86" xr:uid="{FF35CFF0-BA53-4FB5-A429-697A5593F904}"/>
     <cellStyle name="Heading 4" xfId="87" xr:uid="{604A9B68-26AA-42E4-BD59-74F275BDF938}"/>
+    <cellStyle name="Hipervínculo" xfId="156" builtinId="8"/>
     <cellStyle name="Hipervínculo 2" xfId="7" xr:uid="{358A1CFB-C237-483B-8D91-F62099577D0A}"/>
-    <cellStyle name="Hyperlink" xfId="156" builtinId="8"/>
     <cellStyle name="Incorrecto 2" xfId="88" xr:uid="{A05BC124-AD58-4AF9-861D-B4ADC676969B}"/>
     <cellStyle name="Input" xfId="89" xr:uid="{472C1F0D-8989-4A01-991A-5FE66FF8D32E}"/>
     <cellStyle name="Linked Cell" xfId="90" xr:uid="{6DA3D4A1-0660-4453-B217-178166A06AA9}"/>
@@ -1425,9 +1446,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1465,7 +1486,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1571,7 +1592,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1713,7 +1734,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1724,19 +1745,19 @@
   <dimension ref="A1:AM26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="34" style="16" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="16"/>
+    <col min="2" max="2" width="32.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="34" style="15" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="15"/>
     <col min="9" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="16" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="15" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="25.42578125" customWidth="1"/>
     <col min="14" max="14" width="31.5703125" customWidth="1"/>
@@ -1755,25 +1776,25 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -1782,7 +1803,7 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="18" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -1854,7 +1875,7 @@
       <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="26" t="s">
+      <c r="AI1" s="25" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="5" t="s">
@@ -1870,257 +1891,257 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:39" ht="15.75" thickTop="1">
+      <c r="A2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="R2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="S2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="U2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="W2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE2" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF2" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="AG2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI2" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM2" s="36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" ht="54">
+      <c r="A3" s="11">
+        <v>10</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE2" s="9" t="s">
+      <c r="C3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="AF2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI2" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM2" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" ht="49.5">
-      <c r="A3" s="12">
-        <v>701</v>
-      </c>
-      <c r="B3" s="18" t="s">
+      <c r="D3" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="E3" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="24">
+        <v>0</v>
+      </c>
+      <c r="G3" s="23">
+        <v>11</v>
+      </c>
+      <c r="H3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="I3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="J3" s="11">
+        <v>3</v>
+      </c>
+      <c r="K3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="25">
+      <c r="L3" s="11">
         <v>0</v>
       </c>
-      <c r="G3" s="24">
-        <v>11</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="12">
-        <v>3</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="12">
-        <v>0</v>
-      </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <v>120000</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="11">
         <v>400000000</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="26">
         <f>1-(P3/N3)</f>
         <v>5.5000000000000049E-2</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="11">
         <v>378000000</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="11">
         <v>1987</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="11">
         <v>12</v>
       </c>
-      <c r="S3" s="12">
+      <c r="S3" s="11">
         <v>3</v>
       </c>
-      <c r="T3" s="12">
+      <c r="T3" s="11">
         <v>0</v>
       </c>
-      <c r="U3" s="12">
-        <v>85</v>
-      </c>
-      <c r="V3" s="12">
+      <c r="U3" s="11">
+        <v>100.2</v>
+      </c>
+      <c r="V3" s="11">
         <v>1</v>
       </c>
-      <c r="W3" s="12">
+      <c r="W3" s="11">
         <v>1</v>
       </c>
-      <c r="X3" s="12">
+      <c r="X3" s="11">
         <v>1</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Y3" s="11">
         <v>16000000</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="Z3" s="11">
         <v>7000000</v>
       </c>
-      <c r="AA3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB3" s="12">
+      <c r="AA3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB3" s="11">
         <v>4.6857309999999996</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AC3" s="11">
         <v>-74.084351999999996</v>
       </c>
-      <c r="AD3" s="12">
+      <c r="AD3" s="11">
         <v>2</v>
       </c>
-      <c r="AE3" s="14">
+      <c r="AE3" s="13">
         <v>44524</v>
       </c>
-      <c r="AF3" s="12">
+      <c r="AF3" s="11">
         <v>1</v>
       </c>
-      <c r="AG3" s="12">
+      <c r="AG3" s="11">
         <v>314567874</v>
       </c>
-      <c r="AH3" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI3" s="12">
+      <c r="AH3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI3" s="11">
         <v>0.12</v>
       </c>
-      <c r="AJ3" s="12">
+      <c r="AJ3" s="11">
         <v>280000000</v>
       </c>
-      <c r="AK3" s="12">
+      <c r="AK3" s="11">
         <v>9</v>
       </c>
-      <c r="AL3" s="12">
+      <c r="AL3" s="11">
         <v>2</v>
       </c>
-      <c r="AM3" s="12">
+      <c r="AM3" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:39">
       <c r="A4" s="8"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="20"/>
+      <c r="K4" s="19"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
@@ -2152,16 +2173,16 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="8"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="20"/>
+      <c r="K5" s="19"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -2193,16 +2214,16 @@
     </row>
     <row r="6" spans="1:39">
       <c r="A6" s="8"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="20"/>
+      <c r="K6" s="19"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -2234,16 +2255,16 @@
     </row>
     <row r="7" spans="1:39">
       <c r="A7" s="8"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="20"/>
+      <c r="K7" s="19"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
@@ -2275,16 +2296,16 @@
     </row>
     <row r="8" spans="1:39">
       <c r="A8" s="8"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="20"/>
+      <c r="K8" s="19"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -2316,16 +2337,16 @@
     </row>
     <row r="9" spans="1:39">
       <c r="A9" s="8"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="20"/>
+      <c r="K9" s="19"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -2357,16 +2378,16 @@
     </row>
     <row r="10" spans="1:39">
       <c r="A10" s="8"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="20"/>
+      <c r="K10" s="19"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
@@ -2398,16 +2419,16 @@
     </row>
     <row r="11" spans="1:39">
       <c r="A11" s="8"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="20"/>
+      <c r="K11" s="19"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -2439,16 +2460,16 @@
     </row>
     <row r="12" spans="1:39">
       <c r="A12" s="8"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="20"/>
+      <c r="K12" s="19"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
@@ -2480,16 +2501,16 @@
     </row>
     <row r="13" spans="1:39">
       <c r="A13" s="8"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="20"/>
+      <c r="K13" s="19"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
@@ -2521,16 +2542,16 @@
     </row>
     <row r="14" spans="1:39">
       <c r="A14" s="8"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="20"/>
+      <c r="K14" s="19"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -2562,16 +2583,16 @@
     </row>
     <row r="15" spans="1:39">
       <c r="A15" s="8"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="20"/>
+      <c r="K15" s="19"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -2603,16 +2624,16 @@
     </row>
     <row r="16" spans="1:39">
       <c r="A16" s="8"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="8"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="20"/>
+      <c r="K16" s="19"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
@@ -2644,16 +2665,16 @@
     </row>
     <row r="17" spans="1:39">
       <c r="A17" s="8"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="20"/>
+      <c r="K17" s="19"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -2685,16 +2706,16 @@
     </row>
     <row r="18" spans="1:39">
       <c r="A18" s="8"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="20"/>
+      <c r="K18" s="19"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
@@ -2743,14 +2764,14 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" style="16" customWidth="1"/>
-    <col min="4" max="5" width="27.140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="15" customWidth="1"/>
+    <col min="4" max="5" width="27.140625" style="15" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="9" max="10" width="17.5703125" customWidth="1"/>
     <col min="11" max="11" width="24.28515625" customWidth="1"/>
@@ -2770,18 +2791,18 @@
   <sheetData>
     <row r="1" spans="1:32" ht="46.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2818,16 +2839,16 @@
         <v>16</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>26</v>
@@ -2866,209 +2887,209 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
-      <c r="A2" s="1" t="s">
-        <v>39</v>
+    <row r="2" spans="1:32" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A2" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="Z2" s="5" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" s="11" t="s">
-        <v>41</v>
+        <v>87</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF2" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="91.5">
-      <c r="A3" s="12">
-        <v>702</v>
+        <v>88</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="105.75" thickTop="1">
+      <c r="A3" s="11">
+        <v>21</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>11</v>
+      </c>
+      <c r="H3" s="27">
+        <v>11001</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="11">
+        <v>3</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="L3" s="11">
         <v>0</v>
       </c>
-      <c r="G3" s="12">
-        <v>11</v>
-      </c>
-      <c r="H3" s="34">
-        <v>11001</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="12">
-        <v>3</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" s="12">
-        <v>0</v>
-      </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <v>470000000</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="11">
         <f>1-(O3/M3)</f>
         <v>4.2553191489361653E-2</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="11">
         <v>450000000</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="11">
         <v>1990</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="11">
         <v>182</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="11">
         <v>250</v>
       </c>
-      <c r="S3" s="12">
+      <c r="S3" s="11">
         <v>832000</v>
       </c>
-      <c r="T3" s="12">
+      <c r="T3" s="11">
         <v>1250000</v>
       </c>
-      <c r="U3" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="V3" s="12">
+      <c r="U3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="V3" s="11">
         <v>4.6885289999999999</v>
       </c>
-      <c r="W3" s="12">
+      <c r="W3" s="11">
         <v>-74.082549999999998</v>
       </c>
-      <c r="X3" s="12">
+      <c r="X3" s="11">
         <v>2</v>
       </c>
-      <c r="Y3" s="14">
+      <c r="Y3" s="13">
         <v>44524</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="Z3" s="11">
         <v>1</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AA3" s="11">
         <v>3192514878</v>
       </c>
-      <c r="AB3" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC3" s="12">
+      <c r="AB3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC3" s="11">
         <v>320000000</v>
       </c>
-      <c r="AD3" s="12">
+      <c r="AD3" s="11">
         <v>7</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AE3" s="11">
         <v>2</v>
       </c>
-      <c r="AF3" s="12">
+      <c r="AF3" s="11">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="8"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -3099,10 +3120,10 @@
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="8"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -3133,10 +3154,10 @@
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="8"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -3167,10 +3188,10 @@
     </row>
     <row r="7" spans="1:32">
       <c r="A7" s="8"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -3201,10 +3222,10 @@
     </row>
     <row r="8" spans="1:32">
       <c r="A8" s="8"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -3235,10 +3256,10 @@
     </row>
     <row r="9" spans="1:32">
       <c r="A9" s="8"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -3269,10 +3290,10 @@
     </row>
     <row r="10" spans="1:32">
       <c r="A10" s="8"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -3303,10 +3324,10 @@
     </row>
     <row r="11" spans="1:32">
       <c r="A11" s="8"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -3337,10 +3358,10 @@
     </row>
     <row r="12" spans="1:32">
       <c r="A12" s="8"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -3371,10 +3392,10 @@
     </row>
     <row r="13" spans="1:32">
       <c r="A13" s="8"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -3405,10 +3426,10 @@
     </row>
     <row r="14" spans="1:32">
       <c r="A14" s="8"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -3439,10 +3460,10 @@
     </row>
     <row r="15" spans="1:32">
       <c r="A15" s="8"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -3473,10 +3494,10 @@
     </row>
     <row r="16" spans="1:32">
       <c r="A16" s="8"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -3507,10 +3528,10 @@
     </row>
     <row r="17" spans="1:32">
       <c r="A17" s="8"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -3541,10 +3562,10 @@
     </row>
     <row r="18" spans="1:32">
       <c r="A18" s="8"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -3582,15 +3603,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368E751D-99CD-4E38-83A7-64DDA17168D8}">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="40.140625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" style="16" customWidth="1"/>
-    <col min="4" max="5" width="26.28515625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" style="15" customWidth="1"/>
+    <col min="4" max="5" width="26.28515625" style="15" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
     <col min="9" max="10" width="16.7109375" customWidth="1"/>
@@ -3612,18 +3633,18 @@
   <sheetData>
     <row r="1" spans="1:35" ht="46.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -3636,13 +3657,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -3663,16 +3684,16 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>26</v>
@@ -3711,233 +3732,233 @@
         <v>38</v>
       </c>
       <c r="AH1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="15.75" thickTop="1">
+      <c r="A2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="R2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="S2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="U2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z2" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC2" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI2" s="36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="105">
+      <c r="A3" s="11">
+        <v>16</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="E3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>11</v>
+      </c>
+      <c r="H3" s="27">
+        <v>11001</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:35">
-      <c r="A2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI2" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="106.5">
-      <c r="A3" s="12">
-        <v>703</v>
-      </c>
-      <c r="B3" s="18" t="s">
+      <c r="J3" s="11">
+        <v>3</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="L3" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="M3" s="11">
         <v>0</v>
       </c>
-      <c r="G3" s="12">
-        <v>11</v>
-      </c>
-      <c r="H3" s="34">
-        <v>11001</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="J3" s="12">
-        <v>3</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="M3" s="12">
-        <v>0</v>
-      </c>
-      <c r="N3" s="12">
+      <c r="N3" s="11">
         <v>250000000</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="11">
         <f>1-(P3/N3)</f>
         <v>7.999999999999996E-2</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="11">
         <v>230000000</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="11">
         <v>2000</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="11">
         <v>8.5</v>
       </c>
-      <c r="S3" s="12">
+      <c r="S3" s="11">
         <v>200</v>
       </c>
-      <c r="T3" s="12">
+      <c r="T3" s="11">
         <v>875000</v>
       </c>
-      <c r="U3" s="12">
+      <c r="U3" s="11">
         <v>5500000</v>
       </c>
-      <c r="V3" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="W3" s="12">
+      <c r="V3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="W3" s="11">
         <v>3.452655</v>
       </c>
-      <c r="X3" s="12">
+      <c r="X3" s="11">
         <v>-75.471118000000004</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Y3" s="11">
         <v>2</v>
       </c>
-      <c r="Z3" s="14">
+      <c r="Z3" s="13">
         <v>44524</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AA3" s="11">
         <v>1</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AB3" s="11">
         <v>3203135121</v>
       </c>
-      <c r="AC3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD3" s="12">
+      <c r="AC3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD3" s="11">
         <v>185000000</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AE3" s="11">
         <v>2</v>
       </c>
-      <c r="AF3" s="12">
+      <c r="AF3" s="11">
         <v>2</v>
       </c>
-      <c r="AG3" s="12">
+      <c r="AG3" s="11">
         <v>4</v>
       </c>
-      <c r="AH3" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI3" s="12" t="s">
-        <v>60</v>
+      <c r="AH3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI3" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4" s="8"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -3971,10 +3992,10 @@
     </row>
     <row r="5" spans="1:35">
       <c r="A5" s="8"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -4008,10 +4029,10 @@
     </row>
     <row r="6" spans="1:35">
       <c r="A6" s="8"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -4045,10 +4066,10 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" s="8"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -4082,10 +4103,10 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" s="8"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -4119,10 +4140,10 @@
     </row>
     <row r="9" spans="1:35">
       <c r="A9" s="8"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -4156,10 +4177,10 @@
     </row>
     <row r="10" spans="1:35">
       <c r="A10" s="8"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -4193,10 +4214,10 @@
     </row>
     <row r="11" spans="1:35">
       <c r="A11" s="8"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -4230,10 +4251,10 @@
     </row>
     <row r="12" spans="1:35">
       <c r="A12" s="8"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -4267,10 +4288,10 @@
     </row>
     <row r="13" spans="1:35">
       <c r="A13" s="8"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -4304,10 +4325,10 @@
     </row>
     <row r="14" spans="1:35">
       <c r="A14" s="8"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -4341,10 +4362,10 @@
     </row>
     <row r="15" spans="1:35">
       <c r="A15" s="8"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -4378,10 +4399,10 @@
     </row>
     <row r="16" spans="1:35">
       <c r="A16" s="8"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -4415,10 +4436,10 @@
     </row>
     <row r="17" spans="1:35">
       <c r="A17" s="8"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -4452,10 +4473,10 @@
     </row>
     <row r="18" spans="1:35">
       <c r="A18" s="8"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -4489,10 +4510,10 @@
     </row>
     <row r="19" spans="1:35">
       <c r="A19" s="8"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -4526,10 +4547,10 @@
     </row>
     <row r="20" spans="1:35">
       <c r="A20" s="8"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -4563,10 +4584,10 @@
     </row>
     <row r="21" spans="1:35">
       <c r="A21" s="8"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -4600,10 +4621,10 @@
     </row>
     <row r="22" spans="1:35">
       <c r="A22" s="8"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -4637,10 +4658,10 @@
     </row>
     <row r="23" spans="1:35">
       <c r="A23" s="8"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -4674,10 +4695,10 @@
     </row>
     <row r="24" spans="1:35">
       <c r="A24" s="8"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -4711,10 +4732,10 @@
     </row>
     <row r="25" spans="1:35">
       <c r="A25" s="8"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -4761,64 +4782,64 @@
       <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="147.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="29"/>
+    </row>
+    <row r="3" spans="2:3" ht="53.25" customHeight="1">
+      <c r="B3" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="30"/>
+    </row>
+    <row r="4" spans="2:3" ht="168.6" customHeight="1">
+      <c r="B4" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="30"/>
+    </row>
+    <row r="5" spans="2:3" ht="33" customHeight="1" thickBot="1">
+      <c r="B5" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="2:3">
-      <c r="B2" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="30"/>
-    </row>
-    <row r="3" spans="2:3" ht="53.25" customHeight="1">
-      <c r="B3" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="31"/>
-    </row>
-    <row r="4" spans="2:3" ht="168.6" customHeight="1">
-      <c r="B4" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="31"/>
-    </row>
-    <row r="5" spans="2:3" ht="33" customHeight="1" thickBot="1">
-      <c r="B5" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="33"/>
+      <c r="C5" s="32"/>
     </row>
     <row r="6" spans="2:3" ht="40.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="140.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="B7" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="B8" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickTop="1"/>
@@ -5107,13 +5128,41 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73EEC37-EB80-431F-8B64-F31C763C4BAB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73EEC37-EB80-431F-8B64-F31C763C4BAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="56e6d1e7-6899-430c-9877-67183cfe1730"/>
+    <ds:schemaRef ds:uri="12ae8c1a-628e-4358-b6c7-76504a3ed5f5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C102D0FB-C0FD-414E-8250-B5D9BC643251}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C102D0FB-C0FD-414E-8250-B5D9BC643251}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD8AB240-860F-4346-914B-6310FB13AD9E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD8AB240-860F-4346-914B-6310FB13AD9E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="56e6d1e7-6899-430c-9877-67183cfe1730"/>
+    <ds:schemaRef ds:uri="12ae8c1a-628e-4358-b6c7-76504a3ed5f5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Fix: Ajuste de validador e insert ofertas PH, NPH y Rural"
This reverts commit d22f63fc89fa1391255335e7af3416078befb0d0.
</commit_message>
<xml_diff>
--- a/src/files/EJEMPLO_FORMATO_MERCADO_OBSERVATORIO_INMOBILIARIO_NACIONAL.xlsx
+++ b/src/files/EJEMPLO_FORMATO_MERCADO_OBSERVATORIO_INMOBILIARIO_NACIONAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://danegovco-my.sharepoint.com/personal/pagoenagac_dane_gov_co/Documents/Documentos/PAGOENAGAC/02_Observatorio Inmobiliario - OIN/01_Cargues Observadores/Formatos - instructivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{9A1D7074-A131-4087-9D51-A373EB1C5D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F26C8CFA-F316-4B14-B393-0FFF6F70D005}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{9A1D7074-A131-4087-9D51-A373EB1C5D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D99B3FD-3691-4F87-8A3F-0B95BBA50556}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7AEC964B-7FBA-4D6E-B96B-7AAA67EE11BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" xr2:uid="{7AEC964B-7FBA-4D6E-B96B-7AAA67EE11BC}"/>
   </bookViews>
   <sheets>
     <sheet name="PH" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="91">
   <si>
     <t>ID_OFERTA_PH</t>
   </si>
@@ -158,6 +158,12 @@
     <t>TIPO_TIPOLOGIA</t>
   </si>
   <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Dominio</t>
+  </si>
+  <si>
     <t>Number</t>
   </si>
   <si>
@@ -173,6 +179,9 @@
     <t>178956789123</t>
   </si>
   <si>
+    <t>Vacio</t>
+  </si>
+  <si>
     <t>11001</t>
   </si>
   <si>
@@ -201,6 +210,9 @@
   </si>
   <si>
     <t>VR_M2_TERRENO</t>
+  </si>
+  <si>
+    <t>11001011000250034001</t>
   </si>
   <si>
     <t>110010110001700250034001000000</t>
@@ -376,46 +388,28 @@
   <si>
     <t xml:space="preserve">El campo puede estar diligenciado o no. </t>
   </si>
-  <si>
-    <t>Texto</t>
-  </si>
-  <si>
-    <t>Número</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>BDU0001CMJD</t>
-  </si>
-  <si>
-    <t>BDU0001KPJB</t>
-  </si>
-  <si>
-    <t>BCY0001SXJB</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="16">
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;\ * #,##0_);_(&quot;$&quot;\ * \(#,##0\);_(&quot;$&quot;\ * &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="172" formatCode="&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="173" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ "/>
-    <numFmt numFmtId="174" formatCode="&quot;$&quot;\ #,##0.00;[Red]&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="175" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="170" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;\ * #,##0_);_(&quot;$&quot;\ * \(#,##0\);_(&quot;$&quot;\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="173" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="175" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="177" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ "/>
+    <numFmt numFmtId="178" formatCode="&quot;$&quot;\ #,##0.00;[Red]&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="179" formatCode="0.000"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -969,13 +963,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1025,19 +1019,19 @@
     <xf numFmtId="0" fontId="12" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1046,8 +1040,8 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1057,31 +1051,31 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="174" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -1090,7 +1084,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="175" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyFill="0"/>
@@ -1121,27 +1115,27 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="27" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1164,6 +1158,9 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="156"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="26" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="27" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1210,13 +1207,13 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="27" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1231,29 +1228,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="26" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="27" fillId="26" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="174">
@@ -1335,8 +1314,8 @@
     <cellStyle name="Heading 2" xfId="85" xr:uid="{6CAAA471-A847-4956-B6F2-F1B66EE7AE12}"/>
     <cellStyle name="Heading 3" xfId="86" xr:uid="{FF35CFF0-BA53-4FB5-A429-697A5593F904}"/>
     <cellStyle name="Heading 4" xfId="87" xr:uid="{604A9B68-26AA-42E4-BD59-74F275BDF938}"/>
-    <cellStyle name="Hipervínculo" xfId="156" builtinId="8"/>
     <cellStyle name="Hipervínculo 2" xfId="7" xr:uid="{358A1CFB-C237-483B-8D91-F62099577D0A}"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8"/>
     <cellStyle name="Incorrecto 2" xfId="88" xr:uid="{A05BC124-AD58-4AF9-861D-B4ADC676969B}"/>
     <cellStyle name="Input" xfId="89" xr:uid="{472C1F0D-8989-4A01-991A-5FE66FF8D32E}"/>
     <cellStyle name="Linked Cell" xfId="90" xr:uid="{6DA3D4A1-0660-4453-B217-178166A06AA9}"/>
@@ -1446,9 +1425,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1486,7 +1465,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1592,7 +1571,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1734,7 +1713,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1745,19 +1724,19 @@
   <dimension ref="A1:AM26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="34" style="15" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="15"/>
+    <col min="2" max="2" width="32.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="34" style="16" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="16"/>
     <col min="9" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="16" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="25.42578125" customWidth="1"/>
     <col min="14" max="14" width="31.5703125" customWidth="1"/>
@@ -1776,25 +1755,25 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -1803,7 +1782,7 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="19" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -1875,7 +1854,7 @@
       <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="25" t="s">
+      <c r="AI1" s="26" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="5" t="s">
@@ -1891,257 +1870,257 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15.75" thickTop="1">
-      <c r="A2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="P2" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="R2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="T2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="U2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="V2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="W2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="X2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE2" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF2" s="36" t="s">
+    <row r="2" spans="1:39" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AG2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI2" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="AL2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="AM2" s="36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" ht="54">
-      <c r="A3" s="11">
-        <v>10</v>
-      </c>
-      <c r="B3" s="17" t="s">
+      <c r="B2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="K2" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="AF2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI2" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM2" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" ht="49.5">
+      <c r="A3" s="12">
+        <v>701</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="24">
+      <c r="C3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="25">
         <v>0</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="24">
         <v>11</v>
       </c>
-      <c r="H3" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="11">
+      <c r="H3" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="12">
         <v>3</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="11">
+      <c r="K3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="12">
         <v>0</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="12">
         <v>120000</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="12">
         <v>400000000</v>
       </c>
-      <c r="O3" s="26">
+      <c r="O3" s="29">
         <f>1-(P3/N3)</f>
         <v>5.5000000000000049E-2</v>
       </c>
-      <c r="P3" s="11">
+      <c r="P3" s="12">
         <v>378000000</v>
       </c>
-      <c r="Q3" s="11">
+      <c r="Q3" s="12">
         <v>1987</v>
       </c>
-      <c r="R3" s="11">
+      <c r="R3" s="12">
         <v>12</v>
       </c>
-      <c r="S3" s="11">
+      <c r="S3" s="12">
         <v>3</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="12">
         <v>0</v>
       </c>
-      <c r="U3" s="11">
-        <v>100.2</v>
-      </c>
-      <c r="V3" s="11">
+      <c r="U3" s="12">
+        <v>85</v>
+      </c>
+      <c r="V3" s="12">
         <v>1</v>
       </c>
-      <c r="W3" s="11">
+      <c r="W3" s="12">
         <v>1</v>
       </c>
-      <c r="X3" s="11">
+      <c r="X3" s="12">
         <v>1</v>
       </c>
-      <c r="Y3" s="11">
+      <c r="Y3" s="12">
         <v>16000000</v>
       </c>
-      <c r="Z3" s="11">
+      <c r="Z3" s="12">
         <v>7000000</v>
       </c>
-      <c r="AA3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB3" s="11">
+      <c r="AA3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="12">
         <v>4.6857309999999996</v>
       </c>
-      <c r="AC3" s="11">
+      <c r="AC3" s="12">
         <v>-74.084351999999996</v>
       </c>
-      <c r="AD3" s="11">
+      <c r="AD3" s="12">
         <v>2</v>
       </c>
-      <c r="AE3" s="13">
+      <c r="AE3" s="14">
         <v>44524</v>
       </c>
-      <c r="AF3" s="11">
+      <c r="AF3" s="12">
         <v>1</v>
       </c>
-      <c r="AG3" s="11">
+      <c r="AG3" s="12">
         <v>314567874</v>
       </c>
-      <c r="AH3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI3" s="11">
+      <c r="AH3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI3" s="12">
         <v>0.12</v>
       </c>
-      <c r="AJ3" s="11">
+      <c r="AJ3" s="12">
         <v>280000000</v>
       </c>
-      <c r="AK3" s="11">
+      <c r="AK3" s="12">
         <v>9</v>
       </c>
-      <c r="AL3" s="11">
+      <c r="AL3" s="12">
         <v>2</v>
       </c>
-      <c r="AM3" s="11">
+      <c r="AM3" s="12">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:39">
       <c r="A4" s="8"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="19"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
@@ -2173,16 +2152,16 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="8"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="19"/>
+      <c r="K5" s="20"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -2214,16 +2193,16 @@
     </row>
     <row r="6" spans="1:39">
       <c r="A6" s="8"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="19"/>
+      <c r="K6" s="20"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -2255,16 +2234,16 @@
     </row>
     <row r="7" spans="1:39">
       <c r="A7" s="8"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="19"/>
+      <c r="K7" s="20"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
@@ -2296,16 +2275,16 @@
     </row>
     <row r="8" spans="1:39">
       <c r="A8" s="8"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="19"/>
+      <c r="K8" s="20"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -2337,16 +2316,16 @@
     </row>
     <row r="9" spans="1:39">
       <c r="A9" s="8"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="19"/>
+      <c r="K9" s="20"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -2378,16 +2357,16 @@
     </row>
     <row r="10" spans="1:39">
       <c r="A10" s="8"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="19"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
@@ -2419,16 +2398,16 @@
     </row>
     <row r="11" spans="1:39">
       <c r="A11" s="8"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="19"/>
+      <c r="K11" s="20"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -2460,16 +2439,16 @@
     </row>
     <row r="12" spans="1:39">
       <c r="A12" s="8"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="19"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
@@ -2501,16 +2480,16 @@
     </row>
     <row r="13" spans="1:39">
       <c r="A13" s="8"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="19"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
@@ -2542,16 +2521,16 @@
     </row>
     <row r="14" spans="1:39">
       <c r="A14" s="8"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="19"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -2583,16 +2562,16 @@
     </row>
     <row r="15" spans="1:39">
       <c r="A15" s="8"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="19"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -2624,16 +2603,16 @@
     </row>
     <row r="16" spans="1:39">
       <c r="A16" s="8"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="8"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="19"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
@@ -2665,16 +2644,16 @@
     </row>
     <row r="17" spans="1:39">
       <c r="A17" s="8"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="19"/>
+      <c r="K17" s="20"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -2706,16 +2685,16 @@
     </row>
     <row r="18" spans="1:39">
       <c r="A18" s="8"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="19"/>
+      <c r="K18" s="20"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
@@ -2764,14 +2743,14 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" style="15" customWidth="1"/>
-    <col min="4" max="5" width="27.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="16" customWidth="1"/>
+    <col min="4" max="5" width="27.140625" style="16" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="9" max="10" width="17.5703125" customWidth="1"/>
     <col min="11" max="11" width="24.28515625" customWidth="1"/>
@@ -2791,18 +2770,18 @@
   <sheetData>
     <row r="1" spans="1:32" ht="46.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2839,16 +2818,16 @@
         <v>16</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>26</v>
@@ -2887,209 +2866,209 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A2" s="9" t="s">
-        <v>87</v>
+    <row r="2" spans="1:32">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="X2" s="9" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="Y2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD2" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE2" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF2" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="105.75" thickTop="1">
-      <c r="A3" s="11">
-        <v>21</v>
+      <c r="AE2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="91.5">
+      <c r="A3" s="12">
+        <v>702</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="11">
+        <v>58</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="12">
         <v>0</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="12">
         <v>11</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="34">
         <v>11001</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="11">
+      <c r="I3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="12">
         <v>3</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="11">
+      <c r="K3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="12">
         <v>0</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="12">
         <v>470000000</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="12">
         <f>1-(O3/M3)</f>
         <v>4.2553191489361653E-2</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="12">
         <v>450000000</v>
       </c>
-      <c r="P3" s="11">
+      <c r="P3" s="12">
         <v>1990</v>
       </c>
-      <c r="Q3" s="11">
+      <c r="Q3" s="12">
         <v>182</v>
       </c>
-      <c r="R3" s="11">
+      <c r="R3" s="12">
         <v>250</v>
       </c>
-      <c r="S3" s="11">
+      <c r="S3" s="12">
         <v>832000</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="12">
         <v>1250000</v>
       </c>
-      <c r="U3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="V3" s="11">
+      <c r="U3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" s="12">
         <v>4.6885289999999999</v>
       </c>
-      <c r="W3" s="11">
+      <c r="W3" s="12">
         <v>-74.082549999999998</v>
       </c>
-      <c r="X3" s="11">
+      <c r="X3" s="12">
         <v>2</v>
       </c>
-      <c r="Y3" s="13">
+      <c r="Y3" s="14">
         <v>44524</v>
       </c>
-      <c r="Z3" s="11">
+      <c r="Z3" s="12">
         <v>1</v>
       </c>
-      <c r="AA3" s="11">
+      <c r="AA3" s="12">
         <v>3192514878</v>
       </c>
-      <c r="AB3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC3" s="11">
+      <c r="AB3" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC3" s="12">
         <v>320000000</v>
       </c>
-      <c r="AD3" s="11">
+      <c r="AD3" s="12">
         <v>7</v>
       </c>
-      <c r="AE3" s="11">
+      <c r="AE3" s="12">
         <v>2</v>
       </c>
-      <c r="AF3" s="11">
+      <c r="AF3" s="12">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="8"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -3120,10 +3099,10 @@
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="8"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -3154,10 +3133,10 @@
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="8"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -3188,10 +3167,10 @@
     </row>
     <row r="7" spans="1:32">
       <c r="A7" s="8"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -3222,10 +3201,10 @@
     </row>
     <row r="8" spans="1:32">
       <c r="A8" s="8"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -3256,10 +3235,10 @@
     </row>
     <row r="9" spans="1:32">
       <c r="A9" s="8"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -3290,10 +3269,10 @@
     </row>
     <row r="10" spans="1:32">
       <c r="A10" s="8"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -3324,10 +3303,10 @@
     </row>
     <row r="11" spans="1:32">
       <c r="A11" s="8"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -3358,10 +3337,10 @@
     </row>
     <row r="12" spans="1:32">
       <c r="A12" s="8"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -3392,10 +3371,10 @@
     </row>
     <row r="13" spans="1:32">
       <c r="A13" s="8"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -3426,10 +3405,10 @@
     </row>
     <row r="14" spans="1:32">
       <c r="A14" s="8"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -3460,10 +3439,10 @@
     </row>
     <row r="15" spans="1:32">
       <c r="A15" s="8"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -3494,10 +3473,10 @@
     </row>
     <row r="16" spans="1:32">
       <c r="A16" s="8"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -3528,10 +3507,10 @@
     </row>
     <row r="17" spans="1:32">
       <c r="A17" s="8"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -3562,10 +3541,10 @@
     </row>
     <row r="18" spans="1:32">
       <c r="A18" s="8"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -3603,15 +3582,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368E751D-99CD-4E38-83A7-64DDA17168D8}">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="40.140625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" style="15" customWidth="1"/>
-    <col min="4" max="5" width="26.28515625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" style="16" customWidth="1"/>
+    <col min="4" max="5" width="26.28515625" style="16" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
     <col min="9" max="10" width="16.7109375" customWidth="1"/>
@@ -3633,18 +3612,18 @@
   <sheetData>
     <row r="1" spans="1:35" ht="46.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -3657,13 +3636,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -3684,16 +3663,16 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>26</v>
@@ -3732,233 +3711,233 @@
         <v>38</v>
       </c>
       <c r="AH1" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="AI1" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="15.75" thickTop="1">
-      <c r="A2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="M2" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="N2" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="O2" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="P2" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="T2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="U2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="V2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="W2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="X2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z2" s="33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AA2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC2" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="AE2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI2" s="36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="105">
-      <c r="A3" s="11">
-        <v>16</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="11">
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI2" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="106.5">
+      <c r="A3" s="12">
+        <v>703</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="12">
         <v>0</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="12">
         <v>11</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="34">
         <v>11001</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="J3" s="11">
+      <c r="I3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="12">
         <v>3</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="M3" s="11">
+      <c r="K3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="12">
         <v>0</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="12">
         <v>250000000</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="12">
         <f>1-(P3/N3)</f>
         <v>7.999999999999996E-2</v>
       </c>
-      <c r="P3" s="11">
+      <c r="P3" s="12">
         <v>230000000</v>
       </c>
-      <c r="Q3" s="11">
+      <c r="Q3" s="12">
         <v>2000</v>
       </c>
-      <c r="R3" s="11">
+      <c r="R3" s="12">
         <v>8.5</v>
       </c>
-      <c r="S3" s="11">
+      <c r="S3" s="12">
         <v>200</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="12">
         <v>875000</v>
       </c>
-      <c r="U3" s="11">
+      <c r="U3" s="12">
         <v>5500000</v>
       </c>
-      <c r="V3" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="W3" s="11">
+      <c r="V3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="W3" s="12">
         <v>3.452655</v>
       </c>
-      <c r="X3" s="11">
+      <c r="X3" s="12">
         <v>-75.471118000000004</v>
       </c>
-      <c r="Y3" s="11">
+      <c r="Y3" s="12">
         <v>2</v>
       </c>
-      <c r="Z3" s="13">
+      <c r="Z3" s="14">
         <v>44524</v>
       </c>
-      <c r="AA3" s="11">
+      <c r="AA3" s="12">
         <v>1</v>
       </c>
-      <c r="AB3" s="11">
+      <c r="AB3" s="12">
         <v>3203135121</v>
       </c>
-      <c r="AC3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD3" s="11">
+      <c r="AC3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD3" s="12">
         <v>185000000</v>
       </c>
-      <c r="AE3" s="11">
+      <c r="AE3" s="12">
         <v>2</v>
       </c>
-      <c r="AF3" s="11">
+      <c r="AF3" s="12">
         <v>2</v>
       </c>
-      <c r="AG3" s="11">
+      <c r="AG3" s="12">
         <v>4</v>
       </c>
-      <c r="AH3" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI3" s="11" t="s">
-        <v>56</v>
+      <c r="AH3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI3" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4" s="8"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -3992,10 +3971,10 @@
     </row>
     <row r="5" spans="1:35">
       <c r="A5" s="8"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -4029,10 +4008,10 @@
     </row>
     <row r="6" spans="1:35">
       <c r="A6" s="8"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -4066,10 +4045,10 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" s="8"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -4103,10 +4082,10 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" s="8"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -4140,10 +4119,10 @@
     </row>
     <row r="9" spans="1:35">
       <c r="A9" s="8"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -4177,10 +4156,10 @@
     </row>
     <row r="10" spans="1:35">
       <c r="A10" s="8"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -4214,10 +4193,10 @@
     </row>
     <row r="11" spans="1:35">
       <c r="A11" s="8"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -4251,10 +4230,10 @@
     </row>
     <row r="12" spans="1:35">
       <c r="A12" s="8"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -4288,10 +4267,10 @@
     </row>
     <row r="13" spans="1:35">
       <c r="A13" s="8"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -4325,10 +4304,10 @@
     </row>
     <row r="14" spans="1:35">
       <c r="A14" s="8"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -4362,10 +4341,10 @@
     </row>
     <row r="15" spans="1:35">
       <c r="A15" s="8"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -4399,10 +4378,10 @@
     </row>
     <row r="16" spans="1:35">
       <c r="A16" s="8"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -4436,10 +4415,10 @@
     </row>
     <row r="17" spans="1:35">
       <c r="A17" s="8"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -4473,10 +4452,10 @@
     </row>
     <row r="18" spans="1:35">
       <c r="A18" s="8"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -4510,10 +4489,10 @@
     </row>
     <row r="19" spans="1:35">
       <c r="A19" s="8"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -4547,10 +4526,10 @@
     </row>
     <row r="20" spans="1:35">
       <c r="A20" s="8"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -4584,10 +4563,10 @@
     </row>
     <row r="21" spans="1:35">
       <c r="A21" s="8"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -4621,10 +4600,10 @@
     </row>
     <row r="22" spans="1:35">
       <c r="A22" s="8"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -4658,10 +4637,10 @@
     </row>
     <row r="23" spans="1:35">
       <c r="A23" s="8"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -4695,10 +4674,10 @@
     </row>
     <row r="24" spans="1:35">
       <c r="A24" s="8"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -4732,10 +4711,10 @@
     </row>
     <row r="25" spans="1:35">
       <c r="A25" s="8"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -4782,64 +4761,64 @@
       <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="147.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3">
-      <c r="B1" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="29"/>
+      <c r="B1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="2:3">
-      <c r="B2" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="2:3" ht="53.25" customHeight="1">
-      <c r="B3" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="30"/>
+      <c r="B3" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="2:3" ht="168.6" customHeight="1">
-      <c r="B4" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="30"/>
+      <c r="B4" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" spans="2:3" ht="33" customHeight="1" thickBot="1">
-      <c r="B5" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="32"/>
+      <c r="B5" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="33"/>
     </row>
     <row r="6" spans="2:3" ht="40.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="140.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="B7" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="B8" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickTop="1"/>
@@ -5128,41 +5107,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73EEC37-EB80-431F-8B64-F31C763C4BAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="56e6d1e7-6899-430c-9877-67183cfe1730"/>
-    <ds:schemaRef ds:uri="12ae8c1a-628e-4358-b6c7-76504a3ed5f5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73EEC37-EB80-431F-8B64-F31C763C4BAB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C102D0FB-C0FD-414E-8250-B5D9BC643251}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C102D0FB-C0FD-414E-8250-B5D9BC643251}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD8AB240-860F-4346-914B-6310FB13AD9E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="56e6d1e7-6899-430c-9877-67183cfe1730"/>
-    <ds:schemaRef ds:uri="12ae8c1a-628e-4358-b6c7-76504a3ed5f5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD8AB240-860F-4346-914B-6310FB13AD9E}"/>
 </file>
</xml_diff>